<commit_message>
2nd commit fo excel
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>From</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>Via</t>
+  </si>
+  <si>
+    <t>Test Column</t>
   </si>
 </sst>
 </file>
@@ -363,15 +366,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,29 +384,41 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
         <v>8</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>